<commit_message>
update test and mod
</commit_message>
<xml_diff>
--- a/src/output/survey/2-preprocess/all-preprocessed.xlsx
+++ b/src/output/survey/2-preprocess/all-preprocessed.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>software organization,property,software functional property,software,formal method,it engineer,security</t>
+          <t>software,formal method,property,security,software organization,software functional property,it engineer</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>human-centered compute,empirical study in collaborative,collaborative,social compute</t>
+          <t>social compute,collaborative,empirical study in collaborative,human-centered compute</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>computer in other domain,distribute architecture,distribute database transaction,architecture,e-government,data management system,peer-to-peer architecture,computer system organization,apply compute,compute in government,database management system engine,information system</t>
+          <t>computer in other domain,distribute database transaction,database management system engine,distribute architecture,architecture,information system,e-government,apply compute,computer system organization,data management system,compute in government,peer-to-peer architecture</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>compute methodology,distribute compute methodology</t>
+          <t>distribute compute methodology,compute methodology</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>security,privacy</t>
+          <t>privacy,security</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>privacy,social,technology policy,professional topic,compute,security</t>
+          <t>technology policy,privacy,professional topic,social,security,compute</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>general,reference,overview,survey,document type</t>
+          <t>reference,document type,general,overview,survey</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>architecture,computer system organization,peer-to-peer architecture,distribute architecture</t>
+          <t>computer system organization,distribute architecture,architecture,peer-to-peer architecture</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>security,privacy</t>
+          <t>privacy,security</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -924,7 +924,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>embed and cyber-physical system,network property,computer system organization,embed system,network reliability,network</t>
+          <t>network,embed and cyber-physical system,network reliability,computer system organization,network property,embed system</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>network property,network,security</t>
+          <t>security,network,network property</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>general,reference,distribute architecture,overview,architecture,peer-to-peer architecture,privacy,computer system organization,performance,information system,survey,document type,security</t>
+          <t>privacy,security,distribute architecture,performance,information system,architecture,reference,document type,computer system organization,general,overview,survey,peer-to-peer architecture</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>apply compute,enterprise compute</t>
+          <t>enterprise compute,apply compute</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>security,privacy</t>
+          <t>privacy,security</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>general,reference,overview,model of computation,theory of computation,network architecture,network protocol,survey,network,document type</t>
+          <t>network,model of computation,network protocol,reference,document type,theory of computation,general,overview,survey,network architecture</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>general,reference,overview,performance,survey,network,document type</t>
+          <t>network,performance,reference,document type,general,overview,survey</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>web application,network type,wide,world,other logical network structure,information system,online social network,overlay,web,network</t>
+          <t>web application,other logical network structure,network type,wide,network,information system,online social network,overlay,world,web</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>concept map,smart contract,critical analysis,nothing</t>
+          <t>smart contract,concept map,nothing,critical analysis</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,mission critical,performance,quantum compute,computer</t>
+          <t>mission critical,cryptocurrency,computer,performance,bitcoin,quantum compute</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1394,8 +1394,8 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>industrial augmented
-reality,cyber-physical system,big data,nothing,fog,edge compute,industry,industrial iot,compute,smart factory,security</t>
+          <t>industrial iot,industrial augmented
+reality,nothing,smart factory,security,fog,big data,cyber-physical system,industry,compute,edge compute</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>artificial intelligence,wireless communication,irs,index modulation,6g,intelligent reflect surface,terahertz</t>
+          <t>irs,6g,terahertz,artificial intelligence,wireless communication,index modulation,intelligent reflect surface</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>distribute consensus,protocol design,fault tolerance,nothing</t>
+          <t>distribute consensus,fault tolerance,protocol design,nothing</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>theoretical model,analytic model,experiment tool,nothing</t>
+          <t>experiment tool,analytic model,theoretical model,nothing</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>mine management,game theory,security,nothing</t>
+          <t>game theory,security,mine management,nothing</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>cross-chain transaction,nothing,interoperability,ards,st,survey</t>
+          <t>st,nothing,cross-chain transaction,interoperability,ards,survey</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>cooperative robot,distribute control,nothing</t>
+          <t>distribute control,nothing,cooperative robot</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>consensus,permissionless consensus,mine,game theory,p2p network,nothing,incentive mechanism</t>
+          <t>consensus,nothing,permissionless consensus,game theory,incentive mechanism,p2p network,mine</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>security,user privacy,cryptocurrency,bitcoins</t>
+          <t>bitcoins,cryptocurrency,user privacy,security</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>smart contract,cryptocurrency,security,nothing</t>
+          <t>smart contract,cryptocurrency,nothing,security</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>virtual asset,attestation,trust compute,nothing</t>
+          <t>attestation,trust compute,virtual asset,nothing</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>overview,robotics,artificial intelligence,nothing</t>
+          <t>robotics,overview,nothing,artificial intelligence</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>nothing,healthcare,trust,analytics,supply chain,data management,traceability</t>
+          <t>supply chain,data management,nothing,trust,healthcare,traceability,analytics</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptocurrency,nothing,distribute digital ledger,iot</t>
+          <t>consensus,nothing,iot,cryptocurrency,bitcoin,distribute digital ledger</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>nothing,diploma,education,security,certificate</t>
+          <t>education,certificate,nothing,security,diploma</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>consensus,nothing,distribute consensus,dpos,delegate proof of stake</t>
+          <t>consensus,delegate proof of stake,nothing,dpos,distribute consensus</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptography,fault model,concurrent compute,cryptographic protocol,security</t>
+          <t>consensus,security,cryptography,fault model,bitcoin,cryptographic protocol,concurrent compute</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>software define network,uavs,machine learning,d2d communication,nothing,5g network,mobile edge compute,privacy,smart contract,network slice,5g internet of thing,compute,network function virtualization,5g service,security</t>
+          <t>privacy,d2d communication,mobile edge compute,network slice,nothing,smart contract,security,5g internet of thing,5g network,machine learning,5g service,software define network,network function virtualization,uavs,compute</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,system analysis,nothing,design,computer network,smart city,distribute compute,urban sustainability,smart contract,ethereum,crypto token,hyperledger fabric,use case</t>
+          <t>consensus,system analysis,crypto token,nothing,design,distribute compute,smart contract,hyperledger fabric,ethereum,smart city,bitcoin,use case,computer network,urban sustainability,p2p network</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>energy trade,grid 2.0,nothing,distribute energy resource,smart grid,smart contract,microgrid,internet of energy,security,energy internet</t>
+          <t>nothing,smart contract,security,microgrid,energy internet,energy trade,smart grid,internet of energy,grid 2.0,distribute energy resource</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>IoT,industrial application,smart contract,nothing</t>
+          <t>smart contract,industrial application,nothing,iot</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>bitcoin,IoT,edge compute,distribute compute,privacy,performance,autonomous robot,serial digital video out,autonomous system,mobile robot</t>
+          <t>privacy,iot,autonomous robot,mobile robot,distribute compute,performance,serial digital video out,bitcoin,edge compute,autonomous system</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2663,7 +2663,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>nothing,decentralization,software,survey,game</t>
+          <t>software,nothing,game,decentralization,survey</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>game theory,it governance,governance,nash equilibrium,mathematical optimization</t>
+          <t>mathematical optimization,it governance,nash equilibrium,game theory,governance</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>e-government,government technology,digital government,nothing</t>
+          <t>government technology,e-government,digital government,nothing</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>nothing,decentralization,management of science,research data,incentive design</t>
+          <t>incentive design,nothing,research data,decentralization,management of science</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>bitcoin,requirement,embed system</t>
+          <t>requirement,bitcoin,embed system</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>compute,security</t>
+          <t>security,compute</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>machine learning,quantum bite,variational quantum classifier,quantum inspire,hybrid quantum-classical,quantum machine learn,quantum classification,quantum compute</t>
+          <t>quantum machine learn,quantum bite,quantum classification,quantum inspire,machine learning,hybrid quantum-classical,variational quantum classifier,quantum compute</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>relay,http public key pin,cosmos,bitcoin</t>
+          <t>http public key pin,relay,bitcoin,cosmos</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -3039,7 +3039,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>nothing,validators,privacy,e-government system,security,decentralise system</t>
+          <t>privacy,nothing,security,e-government system,validators,decentralise system</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>trade,machine learning,cryptocurrency,econometrics</t>
+          <t>cryptocurrency,trade,econometrics,machine learning</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>program paradigm,bitcoin,ecosystem,stem</t>
+          <t>program paradigm,ecosystem,bitcoin,stem</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>contract defect,empirical study,smart contract,ethereum</t>
+          <t>ethereum,empirical study,contract defect,smart contract</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>tool,debug,nothing,smart contract,solidity,test,ethereum,reproducible bug</t>
+          <t>tool,nothing,smart contract,solidity,ethereum,reproducible bug,test,debug</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>attack surface,peer-to-peer system,security,nothing</t>
+          <t>attack surface,security,peer-to-peer system,nothing</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>dapp,fake news,nothing,decentralization,proof of authenticity,forensics,deepfake,data traceability,security</t>
+          <t>dapp,nothing,security,data traceability,deepfake,decentralization,fake news,proof of authenticity,forensics</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>nothing,empirical study,smart contract,ethereum,software maintenance</t>
+          <t>software maintenance,nothing,empirical study,smart contract,ethereum</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>user experience,bitcoin,cryptocurrency,performance</t>
+          <t>cryptocurrency,bitcoin,performance,user experience</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>machine learning,nothing,technological convergence,artificial intelligence</t>
+          <t>technological convergence,machine learning,nothing,artificial intelligence</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>bitcoin,requirement,global network,distribute compute,essence</t>
+          <t>distribute compute,essence,bitcoin,requirement,global network</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>surface web,cryptocurrency,darknet,illicit drug,deep web,tor-services,security</t>
+          <t>darknet,tor-services,deep web,security,cryptocurrency,illicit drug,surface web</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3647,7 +3647,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>apply cryptography,consensus,nothing,privacy</t>
+          <t>privacy,nothing,apply cryptography,consensus</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>consensus,nothing,privacy,smart contract,security</t>
+          <t>privacy,consensus,nothing,smart contract,security</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>nothing,security,iot</t>
+          <t>security,nothing,iot</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>IoT,machine learning,security,nothing</t>
+          <t>security,machine learning,nothing,iot</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>bitcoin,trace,smart contract,datalog,ethereum,security</t>
+          <t>smart contract,security,ethereum,datalog,bitcoin,trace</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>bitcoin,cryptography,security</t>
+          <t>cryptography,bitcoin,security</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3972,7 +3972,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>nothing,ibc,interoperability</t>
+          <t>ibc,nothing,interoperability</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>nothing,database,decentralization,cap,immutability,acid,dc theorem</t>
+          <t>immutability,nothing,acid,database,dc theorem,decentralization,cap</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,challenge,nothing,motivation,ethereum,survey</t>
+          <t>challenge,nothing,cryptocurrency,ethereum,bitcoin,motivation,survey</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>bitcoin,cryptography,parity bite,smart contract,ethereum,distribute database,power interface,advance configuration,security</t>
+          <t>distribute database,advance configuration,smart contract,security,ethereum,cryptography,bitcoin,parity bite,power interface</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -4207,7 +4207,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>consensus,nothing,IoT,direct acyclic graph,tangle</t>
+          <t>consensus,nothing,iot,tangle,direct acyclic graph</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>selfdestruct function,smart contract,ethereum,empirical study</t>
+          <t>selfdestruct function,empirical study,ethereum,smart contract</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>p2p network,cryptography,database system,distribute database,online bank,tutorial</t>
+          <t>distribute database,database system,online bank,cryptography,tutorial,p2p network</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>p2p network,data mine,cryptography,bibliography,internet,smart contract,online bank</t>
+          <t>bibliography,smart contract,online bank,cryptography,internet,data mine,p2p network</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,smart contract</t>
+          <t>consensus,bitcoin,smart contract</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,microgrids,smart contract,process control,renewable energy source</t>
+          <t>process control,smart contract,renewable energy source,bitcoin,microgrids,p2p network</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>bitcoin,smart contract,p2p network,organization</t>
+          <t>smart contract,p2p network,bitcoin,organization</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,law,smart contract,fault tolerance,fault tolerant system</t>
+          <t>consensus,law,smart contract,fault tolerant system,fault tolerance,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -4583,7 +4583,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,analysis,algorithm design,server,fault tolerance,safety</t>
+          <t>safety,server,fault tolerance,bitcoin,analysis,algorithm design,p2p network</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,medical service,industry,electrical engineer</t>
+          <t>medical service,electrical engineer,industry,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>monitor,p2p network,smart home,smart contract,intelligent sensor,security</t>
+          <t>smart contract,security,intelligent sensor,monitor,smart home,p2p network</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>bank,bitcoin,p2p network,elliptic curve cryptography</t>
+          <t>elliptic curve cryptography,p2p network,bank,bitcoin</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptography,database,ards,st,data structure</t>
+          <t>st,consensus,data structure,database,cryptography,bitcoin,ards</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4818,7 +4818,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>bitcoin,hardware,consensus,data mine,nothing,software</t>
+          <t>software,consensus,nothing,hardware,bitcoin,data mine</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>p2p network,bank,nothing,finance,smart contract,distribute database</t>
+          <t>distribute database,nothing,smart contract,finance,bank,p2p network</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,security</t>
+          <t>security,p2p network,bitcoin</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4959,7 +4959,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,biological system model,server,bay method,computational model</t>
+          <t>nothing,computational model,bay method,biological system model,server,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>IoT,bitcoin,supply chain,smart contract</t>
+          <t>smart contract,supply chain,bitcoin,iot</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>bitcoin,tool,cryptocurrency,nothing,cybercrime investigation,analytics,digital forensics</t>
+          <t>cybercrime investigation,digital forensics,tool,nothing,cryptocurrency,bitcoin,analytics</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -5100,7 +5100,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>IoT,bitcoin,dog,blog</t>
+          <t>dog,bitcoin,blog,iot</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -5147,7 +5147,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,IoT,government</t>
+          <t>nothing,government,iot,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -5194,7 +5194,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>bitcoin,performance,lightning,computer science,plasma</t>
+          <t>computer science,lightning,performance,bitcoin,plasma</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,cryptography,nothing,server,receiver</t>
+          <t>nothing,server,cryptography,bitcoin,receiver,p2p network</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,smart contract,security,authorization</t>
+          <t>nothing,authorization,smart contract,security,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>bitcoin,library,nothing,IoT,systematics,smart contract</t>
+          <t>systematics,nothing,iot,smart contract,bitcoin,library</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>p2p network,cryptography,nothing,smart contract,distribute database,digital forensics</t>
+          <t>digital forensics,distribute database,nothing,smart contract,cryptography,p2p network</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>bitcoin,machine-to-machine communication,nothing,IoT,performance,sensor</t>
+          <t>nothing,iot,performance,sensor,bitcoin,machine-to-machine communication</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>consensus,smart contract,security,nothing</t>
+          <t>consensus,security,smart contract,nothing</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>consensus,cryptocurrency,technological innovation,economics,company</t>
+          <t>consensus,company,cryptocurrency,economics,technological innovation</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -5570,7 +5570,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>p2p network,cryptography,big data,digital signature,IoT</t>
+          <t>iot,big data,digital signature,cryptography,p2p network</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -5617,7 +5617,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,IoT,computer architecture,compute</t>
+          <t>iot,bitcoin,compute,p2p network,computer architecture</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,software,server</t>
+          <t>software,server,p2p network,bitcoin</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>mobile h,dog,privacy,internet,set,security,conference</t>
+          <t>privacy,security,mobile h,set,internet,dog,conference</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>monitor,p2p network,security,collaboration</t>
+          <t>security,p2p network,collaboration,monitor</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -5805,7 +5805,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>market research,bitcoin,consensus,smart contract,fabric,computer language</t>
+          <t>consensus,market research,smart contract,bitcoin,computer language,fabric</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -5852,7 +5852,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>market research,bitcoin,cryptography,information technology,ip network</t>
+          <t>market research,ip network,cryptography,bitcoin,information technology</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -5899,7 +5899,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,proposal,privacy,history</t>
+          <t>privacy,proposal,history,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5946,7 +5946,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,portfolio management,nothing</t>
+          <t>cryptocurrency,portfolio management,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -5993,7 +5993,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>bitcoin,ip network,p2p network,nothing</t>
+          <t>p2p network,ip network,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>investment,bank,cryptocurrency,nothing,economics,control system</t>
+          <t>nothing,cryptocurrency,economics,bank,investment,control system</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -6087,7 +6087,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,cryptography,nothing,tutorial,conference</t>
+          <t>nothing,cryptography,tutorial,bitcoin,conference,p2p network</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>cryptography,nothing,server,medium,plagiarism,watermarking</t>
+          <t>nothing,medium,plagiarism,watermarking,server,cryptography</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>nothing,IoT,augment reality,artificial intelligence,privacy,security,conference</t>
+          <t>privacy,augment reality,nothing,iot,artificial intelligence,security,conference</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -6228,7 +6228,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>market research,nothing,IoT,battery,computer architecture,compute,security</t>
+          <t>nothing,iot,market research,security,battery,compute,computer architecture</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -6275,7 +6275,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>privacy,cryptography,security,nothing</t>
+          <t>privacy,cryptography,nothing,security</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>architecture,structure,type,security</t>
+          <t>security,architecture,structure,type</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -6369,7 +6369,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>bitcoin,smart contract,lake,electronic vote</t>
+          <t>smart contract,bitcoin,electronic vote,lake</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>cryptography,nothing,systematics,smart contract,education,bibliography</t>
+          <t>education,systematics,bibliography,nothing,smart contract,cryptography</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -6463,7 +6463,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptocurrency,pob,nothing,permissioned</t>
+          <t>consensus,nothing,cryptocurrency,permissioned,pob,bitcoin</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>p2p network,oil,nothing,security,distribute database,natural gas,natural gas industry</t>
+          <t>distribute database,nothing,security,natural gas industry,oil,natural gas,p2p network</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -6557,7 +6557,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,security,nothing</t>
+          <t>security,p2p network,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -6604,7 +6604,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>ledger,cryptocurrency,security,nothing</t>
+          <t>ledger,cryptocurrency,nothing,security</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -6651,7 +6651,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>consensus,p2p network,game theory,cryptography,nothing,game</t>
+          <t>consensus,nothing,game,game theory,cryptography,p2p network</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>proposal,bitcoin,privacy,nothing</t>
+          <t>privacy,bitcoin,nothing,proposal</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>consensus,cryptography,nothing,smart grid,industry,renewable energy source</t>
+          <t>consensus,nothing,renewable energy source,industry,cryptography,smart grid</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>nothing,medical service,IoT,industry,software,computer architecture,security</t>
+          <t>software,medical service,nothing,iot,security,industry,computer architecture</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -6886,7 +6886,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>cryptography,nothing,industry,smart contract,organization</t>
+          <t>nothing,smart contract,industry,cryptography,organization</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6933,7 +6933,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>consensus,p2p network,nothing,digital signature,privacy,information technology</t>
+          <t>privacy,consensus,nothing,digital signature,information technology,p2p network</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,nothing,fabric</t>
+          <t>consensus,nothing,bitcoin,p2p network,fabric</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,edge compute,performance,compute</t>
+          <t>nothing,edge compute,performance,bitcoin,compute,p2p network</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -7074,7 +7074,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>machine learning,data mine,nothing,machine learn algorithm,smart contract,decision make</t>
+          <t>nothing,smart contract,machine learning,machine learn algorithm,decision make,data mine</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -7121,7 +7121,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>bitcoin,nothing,government,systematics,smart contract,computer architecture,compute</t>
+          <t>systematics,government,nothing,smart contract,bitcoin,compute,computer architecture</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -7168,7 +7168,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>nothing,IoT,server,technological innovation,interoperability,organization,security</t>
+          <t>nothing,iot,security,server,organization,technological innovation,interoperability</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -7215,7 +7215,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>p2p network,smart contract,industry,government</t>
+          <t>industry,smart contract,p2p network,government</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -7266,7 +7266,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>reliability,law,nothing,smart contract,taxonomy,security</t>
+          <t>law,reliability,nothing,smart contract,security,taxonomy</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -7313,7 +7313,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,digital signature,government,computer architecture</t>
+          <t>nothing,government,digital signature,bitcoin,p2p network,computer architecture</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -7360,7 +7360,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>p2p network,medical service,IoT,industry,smart contract,production</t>
+          <t>medical service,production,iot,smart contract,industry,p2p network</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -7407,7 +7407,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>p2p network,nothing,IoT,database,smart contract,data collection,security</t>
+          <t>data collection,nothing,iot,smart contract,security,database,p2p network</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -7501,7 +7501,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,IoT,smart contract</t>
+          <t>nothing,iot,smart contract,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -7548,7 +7548,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,cryptography,nothing,digital signature,task analysis</t>
+          <t>nothing,task analysis,digital signature,cryptography,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -7595,7 +7595,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>currency,stakeholder,data mine,cryptography,urban area</t>
+          <t>currency,stakeholder,cryptography,data mine,urban area</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -7642,7 +7642,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>IoT,nothing</t>
+          <t>nothing,iot</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -7689,7 +7689,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>p2p network,nothing,sociology,statistic,smart city,security</t>
+          <t>nothing,security,sociology,smart city,statistic,p2p network</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -7736,7 +7736,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>market research,bitcoin,consensus,p2p network,nothing,performance</t>
+          <t>consensus,nothing,market research,performance,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -7783,7 +7783,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>smart home,delay,nothing,IoT,privacy,security</t>
+          <t>privacy,nothing,iot,security,delay,smart home</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -7830,7 +7830,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptography,quantum compute</t>
+          <t>quantum compute,consensus,cryptography,bitcoin</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -7877,7 +7877,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,nothing,smart contract</t>
+          <t>consensus,nothing,smart contract,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -7924,7 +7924,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>nothing,biological system model,automobile,industry,automotive engineer,security</t>
+          <t>nothing,security,automobile,industry,biological system model,automotive engineer</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -7971,7 +7971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>nothing,IoT,task analysis,computer science,bibliography,company</t>
+          <t>computer science,bibliography,nothing,iot,company,task analysis</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,nothing,database,classification algorithm</t>
+          <t>consensus,nothing,database,bitcoin,classification algorithm,p2p network</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>p2p network,cryptography,IoT,medical service,compute</t>
+          <t>medical service,iot,cryptography,compute,p2p network</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -8112,7 +8112,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>nothing,technological innovation,industry,art,smart contract</t>
+          <t>nothing,smart contract,industry,technological innovation,art</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -8159,7 +8159,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>nothing,syntactics,smart contract,security,computational model</t>
+          <t>nothing,smart contract,security,computational model,syntactics</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -8206,7 +8206,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>nothing,IoT,edge compute,smart contract,computer architecture,compute,control system</t>
+          <t>nothing,iot,smart contract,control system,compute,edge compute,computer architecture</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -8253,7 +8253,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,fault tolerance,fault tolerant system</t>
+          <t>consensus,fault tolerant system,fault tolerance,bitcoin</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -8300,7 +8300,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>p2p network,stakeholder,cryptography,nothing,smart contract</t>
+          <t>stakeholder,nothing,smart contract,cryptography,p2p network</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -8394,7 +8394,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>radiofrequency identification,consensus,nothing,IoT,security</t>
+          <t>consensus,nothing,iot,radiofrequency identification,security</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>bitcoin,online bank,server</t>
+          <t>server,online bank,bitcoin</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -8488,7 +8488,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>tutorial,IoT,server,privacy,security</t>
+          <t>privacy,iot,security,server,tutorial</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -8535,7 +8535,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>ehr,nothing,healthcare,survey,phr</t>
+          <t>nothing,phr,healthcare,ehr,survey</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -8582,7 +8582,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>cryptography,nothing,medical service,privacy,compute,biomedical image</t>
+          <t>privacy,medical service,nothing,biomedical image,cryptography,compute</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -8629,7 +8629,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>medical service,bitcoin,smart contract,compute</t>
+          <t>smart contract,medical service,bitcoin,compute</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -8676,7 +8676,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>data structure,bitcoin,smart contract,vegetation</t>
+          <t>smart contract,data structure,vegetation,bitcoin</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -8723,7 +8723,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>p2p network,power market,microgrids,nothing,power system stability,distribute power generation</t>
+          <t>nothing,distribute power generation,power market,power system stability,microgrids,p2p network</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -8770,7 +8770,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>range proof,consensus,nothing,privacy</t>
+          <t>privacy,nothing,range proof,consensus</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -8817,7 +8817,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>bitcoin,systematics,data mine,observer</t>
+          <t>systematics,bitcoin,data mine,observer</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -8864,7 +8864,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,systematics,smart contract</t>
+          <t>systematics,nothing,smart contract,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>consensus,fpga,nothing,cpu,asic,gpu,heterogeneous hardware,hardware architecture</t>
+          <t>fpga,consensus,nothing,asic,cpu,heterogeneous hardware,gpu,hardware architecture</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -8958,7 +8958,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>energy exchange,energy internet,nothing,IoT,energy sector,ecosystem,energy market,energetics,carbon certificate,energy</t>
+          <t>energy market,carbon certificate,iot,nothing,energy exchange,energy internet,ecosystem,energy,energy sector,energetics</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -9005,7 +9005,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,nothing,privacy,history</t>
+          <t>privacy,consensus,nothing,history,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -9052,7 +9052,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>bitcoin,p2p network,nothing,explosive,ip network,online bank</t>
+          <t>nothing,ip network,online bank,explosive,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -9099,7 +9099,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>consensus,p2p network,nothing,systematics,fault tolerance,fault tolerant system</t>
+          <t>consensus,systematics,nothing,fault tolerant system,fault tolerance,p2p network</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -9146,7 +9146,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,security</t>
+          <t>cryptocurrency,bitcoin,security</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -9193,7 +9193,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,privacy,systematics,online bank,bibliography</t>
+          <t>privacy,systematics,consensus,bibliography,online bank,bitcoin</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -9240,7 +9240,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>consensus,nothing,dpos,smart contract,security</t>
+          <t>consensus,nothing,smart contract,security,dpos</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -9287,7 +9287,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>cloud storage,architecture,security,nothing</t>
+          <t>cloud storage,security,architecture,nothing</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -9334,7 +9334,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>p2p network,data model,reliability,nothing,ecosystem,smart contract,fee</t>
+          <t>data model,nothing,reliability,smart contract,fee,ecosystem,p2p network</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -9381,7 +9381,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>compute,decentralization,peer-to -peer network,nothing</t>
+          <t>decentralization,peer-to -peer network,compute,nothing</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -9428,7 +9428,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>p2p network,nothing,systematics,smart contract,supply chain,bibliography</t>
+          <t>systematics,supply chain,bibliography,nothing,smart contract,p2p network</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>p2p network,data mine,nothing,medical service,database,performance,systematics</t>
+          <t>systematics,medical service,nothing,database,performance,data mine,p2p network</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -9522,7 +9522,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>p2p network,smart phone,nothing,performance,task analysis,security</t>
+          <t>nothing,task analysis,security,performance,smart phone,p2p network</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -9569,7 +9569,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>performance,measurement,bitcoin,nothing</t>
+          <t>performance,bitcoin,nothing,measurement</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -9616,7 +9616,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>medical service,industry,privacy,internet,computer architecture</t>
+          <t>privacy,medical service,industry,internet,computer architecture</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>bitcoin,security,nothing</t>
+          <t>security,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -9710,7 +9710,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>market research,bitcoin,nothing,medical service,systematics</t>
+          <t>medical service,systematics,nothing,market research,bitcoin</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -9757,7 +9757,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>nothing,operate system,grid compute,compute,security</t>
+          <t>operate system,grid compute,nothing,security,compute</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -9804,7 +9804,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>cryptocurrency,nothing,supply chain,bibliography,organization</t>
+          <t>bibliography,supply chain,nothing,cryptocurrency,organization</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -9851,7 +9851,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>second layer solution,first layer solution,nothing,sharding,performance</t>
+          <t>nothing,first layer solution,performance,second layer solution,sharding</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>rout,file system,p2p network,width,web server,distribute database,b</t>
+          <t>web server,distribute database,file system,width,b,p2p network,rout</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -9945,7 +9945,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>software define network,p2p network,nothing,software,computer architecture,security,control system</t>
+          <t>software,nothing,security,software define network,control system,p2p network,computer architecture</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -9992,7 +9992,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>reliability,nothing,performance,computer architecture,compute,5g mobile communication,security</t>
+          <t>nothing,reliability,security,performance,5g mobile communication,compute,computer architecture</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -10039,7 +10039,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>hyperledger fabric,nothing,chaincode,hyperledger</t>
+          <t>hyperledger fabric,chaincode,nothing,hyperledger</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -10086,7 +10086,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,p2p network,publish</t>
+          <t>consensus,publish,p2p network,bitcoin</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,privacy</t>
+          <t>privacy,bitcoin,consensus</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -10180,7 +10180,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>IoT,smart city,systematics,bibliography</t>
+          <t>smart city,systematics,bibliography,iot</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
@@ -10274,7 +10274,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>performance,systematic survey,nothing</t>
+          <t>systematic survey,nothing,performance</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -10321,7 +10321,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>consensus,p2p network,nothing,industry,ecosystem,compute,security</t>
+          <t>consensus,nothing,security,industry,ecosystem,compute,p2p network</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -10368,7 +10368,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>big data,nothing,IoT,medical service,edge compute,quality of service,sensor</t>
+          <t>quality of service,medical service,nothing,iot,big data,sensor,edge compute</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -10415,7 +10415,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>cryptography,IoT,privacy,distribute database,data acquisition,performance,pattern classification,compute</t>
+          <t>privacy,data acquisition,distribute database,iot,pattern classification,performance,cryptography,compute</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -10462,7 +10462,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>p2p network,physical layer,nothing,energy resource,australia,energy management,price</t>
+          <t>australia,nothing,energy management,physical layer,energy resource,price,p2p network</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>bitcoin,nothing,smart contract application,smart contract,recent advance in smart contract,smart contract operation</t>
+          <t>smart contract application,recent advance in smart contract,nothing,smart contract,bitcoin,smart contract operation</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -10556,7 +10556,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>p2p network,library,biological system model,adaptation model,education</t>
+          <t>adaptation model,education,biological system model,p2p network,library</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -10603,7 +10603,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>nothing,IoT,smart contract,ethereum,security</t>
+          <t>nothing,iot,smart contract,security,ethereum</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -10650,7 +10650,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>trust-free system,share economy,trust,nothing</t>
+          <t>trust,trust-free system,share economy,nothing</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -10697,7 +10697,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>cryptocurrency,cryptography,nothing,privacy,anonymity</t>
+          <t>privacy,nothing,cryptocurrency,cryptography,anonymity</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -10744,7 +10744,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>mine,cryptocurrency,nothing,privacy,smart contract,security</t>
+          <t>privacy,nothing,smart contract,cryptocurrency,security,mine</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
@@ -10791,7 +10791,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,nothing,IoT,smart contract,security</t>
+          <t>nothing,iot,smart contract,cryptocurrency,security,bitcoin</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
@@ -10838,7 +10838,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>bitcoin,mine,consumption,nothing,energy</t>
+          <t>consumption,nothing,energy,bitcoin,mine</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -10885,7 +10885,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>supply chain,educational background,agriculture sector,nothing</t>
+          <t>agriculture sector,educational background,supply chain,nothing</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -10932,7 +10932,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>bitcoin,smart home,nothing,IoT,transaction,security</t>
+          <t>nothing,iot,security,transaction,bitcoin,smart home</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
@@ -10979,7 +10979,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>prisma-scr,biomedical domain,scoping review,nothing</t>
+          <t>scoping review,prisma-scr,biomedical domain,nothing</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>bitcoin,machine learning,nothing,ethereum,radiology</t>
+          <t>nothing,machine learning,ethereum,bitcoin,radiology</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -11073,7 +11073,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>smart contract,ips2,nothing</t>
+          <t>ips2,smart contract,nothing</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
@@ -11120,7 +11120,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>IoT,data structure,consensus,nothing</t>
+          <t>consensus,data structure,nothing,iot</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
@@ -11167,7 +11167,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>peer-to-peer energy trade,nothing,energy decentralisation,prosumer,renewable energy</t>
+          <t>nothing,renewable energy,peer-to-peer energy trade,prosumer,energy decentralisation</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
@@ -11214,7 +11214,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>nothing,construction industry,socio-technical system,project bank account,compliance,regulation,build environment,use case</t>
+          <t>nothing,regulation,project bank account,use case,socio-technical system,build environment,construction industry,compliance</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -11261,7 +11261,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>IoT,consensus method,hyperledger,nothing</t>
+          <t>hyperledger,consensus method,nothing,iot</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
@@ -11308,7 +11308,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>consensus,permission model,nothing,performance,trust,security</t>
+          <t>consensus,nothing,security,trust,performance,permission model</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -11355,7 +11355,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,price bubble,nothing</t>
+          <t>price bubble,cryptocurrency,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -11449,7 +11449,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>cryptocurrency,decentralize application,nothing,smart contract,digital asset,sidechains,decentralize ledger</t>
+          <t>nothing,smart contract,cryptocurrency,sidechains,digital asset,decentralize ledger,decentralize application</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
@@ -11543,7 +11543,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>merkle tree,cryptography,nothing</t>
+          <t>cryptography,merkle tree,nothing</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -11590,7 +11590,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>correctness,smart contract,security,nothing</t>
+          <t>smart contract,security,correctness,nothing</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
@@ -11637,7 +11637,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>challenge,benefit,nothing,financial technology,functionality</t>
+          <t>benefit,challenge,nothing,functionality,financial technology</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -11684,7 +11684,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>ethical challenge,nothing,ethic,financial industry,adoption</t>
+          <t>ethic,nothing,financial industry,adoption,ethical challenge</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>security,healthcare,benefit,nothing</t>
+          <t>benefit,security,healthcare,nothing</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
@@ -11825,7 +11825,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>nothing,privacy,healthcare,electronic health record system,security</t>
+          <t>privacy,nothing,security,electronic health record system,healthcare</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
@@ -11872,7 +11872,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>consensus,fintech,nothing,innovation,mine industry,z1,o2</t>
+          <t>z1,consensus,nothing,fintech,mine industry,o2,innovation</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -11919,7 +11919,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>food sustainability,nothing,transparency,security,traceability</t>
+          <t>nothing,security,traceability,food sustainability,transparency</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
@@ -11966,7 +11966,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>consensus,nothing,smart community,privacy,smart contract,smart city,security</t>
+          <t>privacy,consensus,nothing,smart community,smart contract,security,smart city</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -12013,7 +12013,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>security,privacy,smart healthcare,nothing</t>
+          <t>privacy,security,smart healthcare,nothing</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -12060,7 +12060,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>health system,scoping review,nothing</t>
+          <t>scoping review,nothing,health system</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -12107,7 +12107,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>machine learning,nothing,IoT,artificial intelligence,security</t>
+          <t>nothing,iot,artificial intelligence,security,machine learning</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -12154,7 +12154,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>nothing,IoT,decentralization,industrial iot,security</t>
+          <t>industrial iot,nothing,iot,security,decentralization</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>nothing,decentralization,cloud exchange,industrial internet of thing,reputation system</t>
+          <t>reputation system,nothing,industrial internet of thing,cloud exchange,decentralization</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
@@ -12248,7 +12248,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>consensus,nothing,smart grid,vehicle-to-grid,internet of energy</t>
+          <t>consensus,nothing,vehicle-to-grid,smart grid,internet of energy</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>nothing,IoT,unman aerial vehicle  network,privacy,security</t>
+          <t>privacy,nothing,iot,security,unman aerial vehicle  network</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -12342,7 +12342,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>nothing,smart grid,industrial iot,e-health,privacy,vanet,supply chain,smart factory,security</t>
+          <t>privacy,industrial iot,vanet,supply chain,nothing,smart factory,security,smart grid,e-health</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -12389,7 +12389,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>adaptive requirement,smart home,nothing,interoperability,smart city,automation,p2p data marketplace,homecare</t>
+          <t>nothing,p2p data marketplace,homecare,adaptive requirement,smart city,automation,interoperability,smart home</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -12436,7 +12436,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>nothing,IoT,privacy,fog compute,5g,security</t>
+          <t>privacy,nothing,iot,fog compute,security,5g</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -12483,7 +12483,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>smart contract,cryptocurrency,security,nothing</t>
+          <t>smart contract,cryptocurrency,nothing,security</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -12577,7 +12577,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>machine learning,nothing,5g network,privacy,5g internet of thing,5g service,security</t>
+          <t>privacy,nothing,security,5g internet of thing,5g network,machine learning,5g service</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -12624,7 +12624,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>bitcoin,nothing,business innovation,computational trust,public ledger</t>
+          <t>nothing,public ledger,computational trust,business innovation,bitcoin</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>decentralization,bank industry transformation,nothing</t>
+          <t>bank industry transformation,nothing,decentralization</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
@@ -12723,7 +12723,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>nothing,equity crowdfunding,transaction,vote of shareholder,regulation of equity crowdfunding,equity registration</t>
+          <t>equity crowdfunding,equity registration,nothing,vote of shareholder,transaction,regulation of equity crowdfunding</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -12773,7 +12773,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>synopsis,p2p platform evolution,new economy,adhocracy,social technology,catallaxies,self-organizing community</t>
+          <t>p2p platform evolution,new economy,social technology,self-organizing community,catallaxies,synopsis,adhocracy</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
@@ -12820,7 +12820,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>om oracle,chain growth,security parameter,network delay,attack strategy,r</t>
+          <t>chain growth,r,network delay,attack strategy,security parameter,om oracle</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>reproducibility,nothing,data share,transparency,privacy</t>
+          <t>privacy,nothing,data share,reproducibility,transparency</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -12917,7 +12917,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>digital currency,business model,disintegration,nothing</t>
+          <t>disintegration,digital currency,nothing,business model</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
@@ -12973,7 +12973,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>sequence,cluster,behavior pattern cluster,nothing</t>
+          <t>cluster,sequence,behavior pattern cluster,nothing</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -13070,7 +13070,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>petri net,model,security,nothing</t>
+          <t>model,security,petri net,nothing</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
@@ -13117,7 +13117,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>asymmetric cryptography,open source software project,financial contract,initial public offer,real money</t>
+          <t>asymmetric cryptography,initial public offer,financial contract,open source software project,real money</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -13164,7 +13164,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>digitalization,research framework,nothing</t>
+          <t>digitalization,nothing,research framework</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>nothing,business model ontology,enterprise ontology,rea</t>
+          <t>enterprise ontology,business model ontology,rea,nothing</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -13308,7 +13308,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>financial service,credit card,financial inclusion,payment system,financial intermediary</t>
+          <t>payment system,credit card,financial inclusion,financial intermediary,financial service</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -13355,7 +13355,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>nothing,decentralize compute,smart contract platform,cod,smart contract program,development</t>
+          <t>decentralize compute,nothing,smart contract program,smart contract platform,development,cod</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>smart contract,ride-hailing service,security,nothing</t>
+          <t>smart contract,security,ride-hailing service,nothing</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -13452,7 +13452,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>self-organisation,consensus,interoperability,nothing,distribute compute,industrial internet of thing,cyber-physical system-of-systems,fault tolerance</t>
+          <t>consensus,nothing,cyber-physical system-of-systems,self-organisation,distribute compute,industrial internet of thing,fault tolerance,interoperability</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -13499,7 +13499,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>food supply chain,case study,nothing</t>
+          <t>case study,food supply chain,nothing</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -13546,7 +13546,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>nothing,mutual fund,performance,ethereum,smart city</t>
+          <t>mutual fund,nothing,performance,ethereum,smart city</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -13594,7 +13594,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>system design,healthcare,holistic approach,nothing</t>
+          <t>holistic approach,healthcare,nothing,system design</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -13641,7 +13641,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>smart contract,legal contract,nothing</t>
+          <t>legal contract,smart contract,nothing</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>information service,consensus,virtual scientific communication,scientific communication,nothing,project management,hash function,information support,scientific</t>
+          <t>consensus,nothing,hash function,virtual scientific communication,scientific communication,information service,project management,information support,scientific</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -13743,7 +13743,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>box,regulatory s,nothing,technology neutrality,initial coin offer,insolvency law</t>
+          <t>nothing,regulatory s,initial coin offer,box,insolvency law,technology neutrality</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -13792,7 +13792,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>verteilte buchführung,consensus,asymmetrische verschlüsselung,konsensalgorithmus,kryptowährung,nothing,distibuted ledger,cryptocurrency,asymmetric encryption</t>
+          <t>consensus,asymmetric encryption,nothing,asymmetrische verschlüsselung,cryptocurrency,distibuted ledger,konsensalgorithmus,verteilte buchführung,kryptowährung</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -13842,7 +13842,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>transaction network,bitcoin adoption,nothing</t>
+          <t>transaction network,nothing,bitcoin adoption</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -13891,7 +13891,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>maritime industry,green supply chain,green it,nothing</t>
+          <t>green supply chain,maritime industry,nothing,green it</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -13938,7 +13938,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>nothing,architecture,information protection,certification,security</t>
+          <t>information protection,nothing,security,architecture,certification</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -13986,7 +13986,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,nothing,quantum mechanic,neuroscience,heisenberg uncertainty principle</t>
+          <t>consensus,nothing,heisenberg uncertainty principle,neuroscience,quantum mechanic,bitcoin</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -14033,7 +14033,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>electric utility,nothing,smart grid,energy sector,business process innovation,energy transformation,smart contract</t>
+          <t>nothing,smart contract,energy sector,smart grid,energy transformation,electric utility,business process innovation</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -14080,7 +14080,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>g21,information asymmetry,g30,nothing,o33,smes finance,credit ration</t>
+          <t>nothing,o33,information asymmetry,credit ration,smes finance,g30,g21</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -14130,7 +14130,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>dapp,nothing,IoT,software architecture,architecture style,smart contract</t>
+          <t>architecture style,dapp,nothing,iot,smart contract,software architecture</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -14177,7 +14177,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>distribute system,decentralize feature,IoT,nothing</t>
+          <t>decentralize feature,distribute system,nothing,iot</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -14225,7 +14225,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>solve complex mathematical problem,nothing,initial coin offer,data marketplace,sale item</t>
+          <t>nothing,initial coin offer,sale item,solve complex mathematical problem,data marketplace</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -14272,7 +14272,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>nothing,citizen broadb,spectrum share,cognitive radio,5g,mobile broadb,radio service</t>
+          <t>mobile broadb,nothing,cognitive radio,5g,citizen broadb,radio service,spectrum share</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -14319,7 +14319,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>initial coin offer,excellent potential application,cryptocurrency,nothing</t>
+          <t>cryptocurrency,excellent potential application,nothing,initial coin offer</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -14413,7 +14413,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>nothing,IoT,smart contract,e-governance,smart place</t>
+          <t>nothing,iot,smart contract,smart place,e-governance</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -14461,7 +14461,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>nothing,smart contract,cryptocurrency exchange,ico,security</t>
+          <t>nothing,smart contract,security,ico,cryptocurrency exchange</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -14556,7 +14556,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>tourism,transparency,trust,nothing</t>
+          <t>transparency,trust,tourism,nothing</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -14603,7 +14603,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>agriculture,nothing</t>
+          <t>nothing,agriculture</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -14650,7 +14650,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>smart home,nothing,food supply chain,critical control point,hazard analysis</t>
+          <t>nothing,hazard analysis,critical control point,smart home,food supply chain</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -14697,7 +14697,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>business,nothing</t>
+          <t>nothing,business</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -14745,7 +14745,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>IoT,privacy,security,nothing</t>
+          <t>privacy,security,nothing,iot</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -14793,7 +14793,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>cryptography,nothing,crypto-spatial coordinate system,IoT,healthcare,smart contract,pharmaceutical,smart city,supply chain,clinical trial</t>
+          <t>supply chain,nothing,iot,crypto-spatial coordinate system,pharmaceutical,smart contract,clinical trial,cryptography,smart city,healthcare</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -14843,7 +14843,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>nothing,patient,healthcare,smart contract,security</t>
+          <t>nothing,smart contract,security,patient,healthcare</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -14890,7 +14890,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>cryptography,data transfer integrity,security,nothing</t>
+          <t>cryptography,data transfer integrity,nothing,security</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -14937,7 +14937,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>mobility,logistics,nothing</t>
+          <t>logistics,mobility,nothing</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -14984,7 +14984,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>bitcoin,block-generation process,nothing,mine process,matrix-geometric solution,process,queue theory</t>
+          <t>matrix-geometric solution,process,block-generation process,nothing,bitcoin,queue theory,mine process</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -15031,7 +15031,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,nothing,smart contract,elliptic curve digital signature algorithm</t>
+          <t>elliptic curve digital signature algorithm,consensus,nothing,smart contract,bitcoin</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -15078,7 +15078,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>nothing,ibe,digital identity</t>
+          <t>ibe,digital identity,nothing</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -15125,7 +15125,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>construction industry,socio-technical system,build environment,nothing</t>
+          <t>socio-technical system,build environment,construction industry,nothing</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -15172,7 +15172,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>supply chain,cryptocurrency,logistics,nothing</t>
+          <t>logistics,cryptocurrency,supply chain,nothing</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>adoption constraint,develop country,nothing</t>
+          <t>develop country,adoption constraint,nothing</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -15267,7 +15267,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>cryptocurrency,csai,nothing,sentiment analysis,forecast,compute,ico</t>
+          <t>csai,nothing,cryptocurrency,sentiment analysis,ico,forecast,compute</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -15314,7 +15314,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>legal framework,cryptocurrency,nothing</t>
+          <t>cryptocurrency,legal framework,nothing</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -15361,7 +15361,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>legal relevance,antlr,nothing,esml,smart contract,ontological completeness,socio-technical</t>
+          <t>antlr,nothing,socio-technical,legal relevance,smart contract,esml,ontological completeness</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -15408,7 +15408,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>cr model,zk-snarks,security,privacy</t>
+          <t>privacy,security,cr model,zk-snarks</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -15456,7 +15456,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>smart contract,digital economy,nothing</t>
+          <t>digital economy,smart contract,nothing</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -15503,7 +15503,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>taxation,electronic document,smart contract,nothing</t>
+          <t>smart contract,taxation,electronic document,nothing</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -15550,7 +15550,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>turing complete language,computability,nothing</t>
+          <t>computability,turing complete language,nothing</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -15597,7 +15597,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>islamic finance,nothing,digital bank,smart contract,islamic trade finance</t>
+          <t>islamic finance,nothing,smart contract,digital bank,islamic trade finance</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -15694,7 +15694,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>consensus,nothing,data share,smart contract,data management</t>
+          <t>consensus,data management,nothing,smart contract,data share</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -15741,7 +15741,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>smart wallet,cost,security,nothing</t>
+          <t>cost,security,smart wallet,nothing</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -15788,7 +15788,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>consensus,proof-of-credibility,decentralize system,nothing</t>
+          <t>decentralize system,consensus,proof-of-credibility,nothing</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -15836,7 +15836,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>electronic health record,nothing,genomics,health informatics,supply chain,healthcare technology,clinical trial,medical licensure</t>
+          <t>genomics,supply chain,nothing,healthcare technology,electronic health record,clinical trial,medical licensure,health informatics</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -15886,7 +15886,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>data mine,fintech,big data,nothing,big data analytics</t>
+          <t>nothing,big data,big data analytics,fintech,data mine</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -15933,7 +15933,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>data store,referential integrity,data access,nothing,privacy,relation</t>
+          <t>privacy,relation,nothing,data store,referential integrity,data access</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -15980,7 +15980,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>access control,nothing,xacml,smart contract,ethereum</t>
+          <t>nothing,xacml,smart contract,access control,ethereum</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -16027,7 +16027,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>architecture,peer-to-peer network,development process</t>
+          <t>peer-to-peer network,development process,architecture</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -16074,7 +16074,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>decentralization,attendance management system,security,nothing</t>
+          <t>attendance management system,security,nothing,decentralization</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -16121,7 +16121,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>linda on corda,smart contract,coordination,linda on ethereum,linda on fabric</t>
+          <t>smart contract,linda on ethereum,linda on corda,coordination,linda on fabric</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
@@ -16263,7 +16263,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>test-driven software development,software development integrity,software production,nothing</t>
+          <t>software production,software development integrity,nothing,test-driven software development</t>
         </is>
       </c>
       <c r="E336" t="inlineStr">
@@ -16310,7 +16310,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>supply chain,transparency,sustainability,nothing</t>
+          <t>transparency,sustainability,supply chain,nothing</t>
         </is>
       </c>
       <c r="E337" t="inlineStr">
@@ -16357,7 +16357,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>the protection of digital copyright,time stamp,hash,nothing</t>
+          <t>hash,the protection of digital copyright,nothing,time stamp</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
@@ -16404,7 +16404,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>machine learning,cryptography,insurance,deep learning,artificial intelligence,nothing,health information exchange,IoT,electronic medical record,emr,hyperledger,pharma,decentralize consensus,robotics,ethereum,pharmacogenomics,precision medicine</t>
+          <t>precision medicine,pharma,deep learning,emr,iot,nothing,robotics,insurance,artificial intelligence,decentralize consensus,pharmacogenomics,machine learning,electronic medical record,ethereum,cryptography,hyperledger,health information exchange</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
@@ -16451,7 +16451,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>space information network,security,nothing</t>
+          <t>security,space information network,nothing</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
@@ -16499,7 +16499,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>certification authority,nothing,decentralize infrastructure,blockstack infrastructure,security</t>
+          <t>nothing,blockstack infrastructure,security,decentralize infrastructure,certification authority</t>
         </is>
       </c>
       <c r="E341" t="inlineStr">
@@ -16549,7 +16549,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>3d animation teach material,nothing,flip learn,role-playing game,emerge technology</t>
+          <t>role-playing game,nothing,flip learn,3d animation teach material,emerge technology</t>
         </is>
       </c>
       <c r="E342" t="inlineStr">
@@ -16596,7 +16596,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>distribute technique,consensus,security,nothing</t>
+          <t>consensus,security,nothing,distribute technique</t>
         </is>
       </c>
       <c r="E343" t="inlineStr">
@@ -16643,7 +16643,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>critical national infrastructure,cyber operation,nothing,data breach,cyberwarfare,scada,healthcare,red team,security</t>
+          <t>critical national infrastructure,cyberwarfare,cyber operation,nothing,data breach,security,scada,red team,healthcare</t>
         </is>
       </c>
       <c r="E344" t="inlineStr">
@@ -16690,7 +16690,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>nothing,aesthetic,smart contract,interactional aesthetic,critical technical practice</t>
+          <t>aesthetic,interactional aesthetic,nothing,smart contract,critical technical practice</t>
         </is>
       </c>
       <c r="E345" t="inlineStr">
@@ -16738,7 +16738,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>naive bay classifier,p2p network,nothing,microlending,hyperledger fabric</t>
+          <t>naive bay classifier,nothing,hyperledger fabric,p2p network,microlending</t>
         </is>
       </c>
       <c r="E346" t="inlineStr">
@@ -16785,7 +16785,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>learn content creation,instructional design,nothing</t>
+          <t>instructional design,learn content creation,nothing</t>
         </is>
       </c>
       <c r="E347" t="inlineStr">
@@ -16832,7 +16832,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,solar energy,nothing,distribute generation,distribute mobility service,photovoltaic,renewable energy,smart contract,microgrid,electric grid,ridesharing,electric vehicle,autonomous vehicle</t>
+          <t>distribute generation,distribute mobility service,solar energy,nothing,photovoltaic,electric vehicle,electric grid,smart contract,microgrid,autonomous vehicle,cryptocurrency,renewable energy,bitcoin,ridesharing</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
@@ -16879,7 +16879,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>consensus,nothing,performance,mean-value analysis,fork-join queue network</t>
+          <t>consensus,mean-value analysis,nothing,performance,fork-join queue network</t>
         </is>
       </c>
       <c r="E349" t="inlineStr">
@@ -16927,7 +16927,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>cryptography,nothing,industry,industrial iot,privacy,supply chain,security</t>
+          <t>privacy,industrial iot,supply chain,nothing,security,industry,cryptography</t>
         </is>
       </c>
       <c r="E350" t="inlineStr">
@@ -16974,7 +16974,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>temporal epistemic logic with probability,nothing,formal model,specification,security,multi-agent system</t>
+          <t>specification,multi-agent system,nothing,security,formal model,temporal epistemic logic with probability</t>
         </is>
       </c>
       <c r="E351" t="inlineStr">
@@ -17069,7 +17069,7 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,security</t>
+          <t>consensus,security,bitcoin</t>
         </is>
       </c>
       <c r="E353" t="inlineStr">
@@ -17164,7 +17164,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>byzantine failure,consensus,replicate system,nothing,state machine replication,fault tolerance</t>
+          <t>consensus,nothing,byzantine failure,state machine replication,fault tolerance,replicate system</t>
         </is>
       </c>
       <c r="E355" t="inlineStr">
@@ -17213,7 +17213,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>digital witness,liability attribution,forensic readiness,digital evidence,e-health,privacy,incident response,digital investigation,decentralise compute</t>
+          <t>digital investigation,privacy,decentralise compute,incident response,digital witness,forensic readiness,digital evidence,e-health,liability attribution</t>
         </is>
       </c>
       <c r="E356" t="inlineStr">
@@ -17260,7 +17260,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>access control,nothing,system chaincode,continuous monitor,usage control</t>
+          <t>nothing,system chaincode,usage control,access control,continuous monitor</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
@@ -17310,7 +17310,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>bitcoin,block-structured markov process,nothing,markovian arrival process,matrix-geometric solution,rg factorization,phase type  distribution</t>
+          <t>block-structured markov process,matrix-geometric solution,markovian arrival process,nothing,phase type  distribution,rg factorization,bitcoin</t>
         </is>
       </c>
       <c r="E358" t="inlineStr">
@@ -17359,7 +17359,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>data management,hospital 4.0,nothing,industrial iot,security</t>
+          <t>industrial iot,data management,nothing,security,hospital 4.0</t>
         </is>
       </c>
       <c r="E359" t="inlineStr">
@@ -17406,7 +17406,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>IoT,distribute system,nothing</t>
+          <t>distribute system,nothing,iot</t>
         </is>
       </c>
       <c r="E360" t="inlineStr">
@@ -17454,7 +17454,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>cad,plm,nothing,privacy,pdm,bim</t>
+          <t>plm,privacy,cad,nothing,bim,pdm</t>
         </is>
       </c>
       <c r="E361" t="inlineStr">
@@ -17548,7 +17548,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>consensus,agent-based model,empirical multiplayer game,nothing</t>
+          <t>consensus,empirical multiplayer game,nothing,agent-based model</t>
         </is>
       </c>
       <c r="E363" t="inlineStr">
@@ -17595,7 +17595,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>decentralize,p2p network,nothing,pharmaceutical supply chain,smart contract</t>
+          <t>decentralize,nothing,pharmaceutical supply chain,smart contract,p2p network</t>
         </is>
       </c>
       <c r="E364" t="inlineStr">
@@ -17642,7 +17642,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>machine learning,cryptocurrency,artificial intelligence,nothing,deep learning,decentralize network</t>
+          <t>decentralize network,deep learning,nothing,artificial intelligence,cryptocurrency,machine learning</t>
         </is>
       </c>
       <c r="E365" t="inlineStr">
@@ -17690,7 +17690,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>scientometric,research cooperation,knowledge map,web of science,lock chain research</t>
+          <t>web of science,knowledge map,lock chain research,research cooperation,scientometric</t>
         </is>
       </c>
       <c r="E366" t="inlineStr">
@@ -17737,7 +17737,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>graph analysis,data mine,nothing,anomaly detection,security</t>
+          <t>nothing,security,graph analysis,data mine,anomaly detection</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
@@ -17833,7 +17833,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>distribute system,cryptocurrency,nothing,technical characteristic,taxonomy</t>
+          <t>technical characteristic,nothing,cryptocurrency,taxonomy,distribute system</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
@@ -17880,7 +17880,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>research,co-authorships,scientometrics,co-occurrence analysis,bibliographic couple</t>
+          <t>co-occurrence analysis,co-authorships,scientometrics,research,bibliographic couple</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
@@ -17927,7 +17927,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>electronic health record,decentralise application,nothing,privacy,healthcare,security</t>
+          <t>privacy,nothing,electronic health record,security,decentralise application,healthcare</t>
         </is>
       </c>
       <c r="E371" t="inlineStr">
@@ -17976,7 +17976,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>supply chain finance,digital economy,security,nothing</t>
+          <t>digital economy,security,supply chain finance,nothing</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
@@ -18023,7 +18023,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>big data,deep learning,nothing,electronic medical record,security</t>
+          <t>deep learning,nothing,security,big data,electronic medical record</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
@@ -18118,7 +18118,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>consensus,efficiency,data overhead,nothing</t>
+          <t>efficiency,consensus,data overhead,nothing</t>
         </is>
       </c>
       <c r="E375" t="inlineStr">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>nothing,privacy,crowdsourcing service,trust,security</t>
+          <t>privacy,nothing,security,trust,crowdsourcing service</t>
         </is>
       </c>
       <c r="E376" t="inlineStr">
@@ -18216,7 +18216,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>IoT,privacy,cryptocurrency,nothing</t>
+          <t>privacy,cryptocurrency,nothing,iot</t>
         </is>
       </c>
       <c r="E377" t="inlineStr">
@@ -18263,7 +18263,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>digital economy,incentive mechanism,nothing</t>
+          <t>incentive mechanism,digital economy,nothing</t>
         </is>
       </c>
       <c r="E378" t="inlineStr">
@@ -18310,7 +18310,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>government-issued electronic identity,eid,nothing</t>
+          <t>eid,government-issued electronic identity,nothing</t>
         </is>
       </c>
       <c r="E379" t="inlineStr">
@@ -18357,7 +18357,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>nothing,trust,supply chain,logistics,traceability</t>
+          <t>supply chain,nothing,trust,traceability,logistics</t>
         </is>
       </c>
       <c r="E380" t="inlineStr">
@@ -18405,7 +18405,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>dpos,consensus,pbft,nothing</t>
+          <t>consensus,pbft,dpos,nothing</t>
         </is>
       </c>
       <c r="E381" t="inlineStr">
@@ -18455,7 +18455,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>performance,consensus,benchmark,nothing</t>
+          <t>benchmark,consensus,nothing,performance</t>
         </is>
       </c>
       <c r="E382" t="inlineStr">
@@ -18502,7 +18502,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>economics,business,citespace,nothing</t>
+          <t>business,economics,nothing,citespace</t>
         </is>
       </c>
       <c r="E383" t="inlineStr">
@@ -18552,7 +18552,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>architecture,computational trust,business innovation,public ledger</t>
+          <t>business innovation,computational trust,public ledger,architecture</t>
         </is>
       </c>
       <c r="E384" t="inlineStr">
@@ -18599,7 +18599,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>nothing,performance,absorptive capacity,start-ups,digital transformation</t>
+          <t>digital transformation,nothing,performance,absorptive capacity,start-ups</t>
         </is>
       </c>
       <c r="E385" t="inlineStr">
@@ -18693,7 +18693,7 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>conceptualization,o39,technology adoption,nothing,terminology</t>
+          <t>terminology,nothing,conceptualization,o39,technology adoption</t>
         </is>
       </c>
       <c r="E387" t="inlineStr">
@@ -18743,7 +18743,7 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>IoT,biot,security,nothing</t>
+          <t>biot,security,nothing,iot</t>
         </is>
       </c>
       <c r="E388" t="inlineStr">
@@ -18793,7 +18793,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>legal issue,nothing,project ecosystem,smart contract,technical</t>
+          <t>nothing,legal issue,smart contract,technical,project ecosystem</t>
         </is>
       </c>
       <c r="E389" t="inlineStr">
@@ -18888,7 +18888,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>loyalty program,nothing,e-commerce,transformation,social shop</t>
+          <t>transformation,nothing,loyalty program,social shop,e-commerce</t>
         </is>
       </c>
       <c r="E391" t="inlineStr">
@@ -18987,7 +18987,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>electronic health record,challenge,e-health,nothing</t>
+          <t>electronic health record,e-health,nothing,challenge</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -19037,7 +19037,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>supply chain,security,nothing</t>
+          <t>security,supply chain,nothing</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -19085,7 +19085,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>distribute system,bitcoin,consensus,nothing</t>
+          <t>bitcoin,consensus,distribute system,nothing</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -19132,7 +19132,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>nothing,smart contract,software engineer</t>
+          <t>smart contract,software engineer,nothing</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -19179,7 +19179,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>his,consensus,nothing,dpos,hyperledger,poa,raft,poet</t>
+          <t>consensus,raft,nothing,poa,dpos,his,hyperledger,poet</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
@@ -19226,7 +19226,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>IoT,nothing</t>
+          <t>nothing,iot</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -19276,7 +19276,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>artificial intelligence,IoT,nothing,smart contract,compute,security</t>
+          <t>nothing,iot,artificial intelligence,smart contract,security,compute</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -19323,7 +19323,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>mechanism,structure,shari’ah,nothing</t>
+          <t>mechanism,structure,nothing,shari’ah</t>
         </is>
       </c>
       <c r="E400" t="inlineStr">
@@ -19370,7 +19370,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>IoT,distribute consensus,nothing</t>
+          <t>distribute consensus,nothing,iot</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -19418,7 +19418,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>consensus,puzzle design,open network protocol,nothing,proof of stack,hybrid consensus</t>
+          <t>consensus,puzzle design,nothing,open network protocol,hybrid consensus,proof of stack</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
@@ -19465,7 +19465,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>distribute system,IoT,security,nothing</t>
+          <t>security,distribute system,nothing,iot</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -19513,7 +19513,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>formal specification,security,nothing</t>
+          <t>security,formal specification,nothing</t>
         </is>
       </c>
       <c r="E404" t="inlineStr">
@@ -19561,7 +19561,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>privacy,biometrics,security,nothing</t>
+          <t>privacy,security,biometrics,nothing</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -19608,7 +19608,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>private chain,implementation,practical insight,nothing</t>
+          <t>implementation,practical insight,nothing,private chain</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -19658,7 +19658,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>IoT,security,nothing</t>
+          <t>security,nothing,iot</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -19705,7 +19705,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>book management,web application,nothing</t>
+          <t>web application,book management,nothing</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -19752,7 +19752,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>consensus,layer architecture,nothing,service-oriented architecture,enterprise service</t>
+          <t>consensus,layer architecture,nothing,enterprise service,service-oriented architecture</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -19799,7 +19799,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>performance,privacy,nothing</t>
+          <t>privacy,nothing,performance</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -19846,7 +19846,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>bitcoin,mine,cryptocurrency,ransomware,nothing,decentralize payment system,monero,smart contract,profitability,ethereum,electronic payment,energy efficiency</t>
+          <t>nothing,energy efficiency,smart contract,electronic payment,cryptocurrency,decentralize payment system,ethereum,ransomware,bitcoin,profitability,mine,monero</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -19940,7 +19940,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>vanet,vehicular adhoc network,security,nothing</t>
+          <t>vehicular adhoc network,security,vanet,nothing</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -19987,7 +19987,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>IoT,iomt,security,nothing</t>
+          <t>iomt,security,nothing,iot</t>
         </is>
       </c>
       <c r="E414" t="inlineStr">
@@ -20035,7 +20035,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>cryptography,hash,nothing,digital signature,algorithm</t>
+          <t>hash,nothing,digital signature,cryptography,algorithm</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -20083,7 +20083,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>IoT,wireless sensor network,security,nothing</t>
+          <t>security,wireless sensor network,nothing,iot</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -20130,7 +20130,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>bitcoin,cryptography,nothing,hyperledger,ethereum</t>
+          <t>nothing,ethereum,cryptography,bitcoin,hyperledger</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -20177,7 +20177,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>ico,cryptocurrency,token,nothing</t>
+          <t>ico,cryptocurrency,nothing,token</t>
         </is>
       </c>
       <c r="E418" t="inlineStr">
@@ -20224,7 +20224,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>bitcoin,mine,cryptocurrency,miner</t>
+          <t>cryptocurrency,miner,mine,bitcoin</t>
         </is>
       </c>
       <c r="E419" t="inlineStr">
@@ -20271,7 +20271,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>nothing,software engineer,development process model,trustless append-only decentralize digital ledger,smart contract,survey,design science</t>
+          <t>design science,nothing,smart contract,trustless append-only decentralize digital ledger,development process model,survey,software engineer</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -20321,7 +20321,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>data analytics,aadhaar authentication,argon2id,digilocker,ethereum,security</t>
+          <t>argon2id,security,ethereum,data analytics,aadhaar authentication,digilocker</t>
         </is>
       </c>
       <c r="E421" t="inlineStr">
@@ -20368,7 +20368,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>cryptoexchanges,cryptocurrency,token offer,nothing</t>
+          <t>cryptocurrency,token offer,nothing,cryptoexchanges</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -20415,7 +20415,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>model-driven engineer,archimate,nothing,hyperledger composer,demo,enterprise engineer</t>
+          <t>enterprise engineer,nothing,archimate,model-driven engineer,hyperledger composer,demo</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -20462,7 +20462,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>transform,dimension,nothing,enterprise,ecommerce application,privacy,trust,security</t>
+          <t>privacy,ecommerce application,nothing,security,trust,dimension,enterprise,transform</t>
         </is>
       </c>
       <c r="E424" t="inlineStr">
@@ -20510,7 +20510,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>IoT,biot,nothing</t>
+          <t>biot,nothing,iot</t>
         </is>
       </c>
       <c r="E425" t="inlineStr">
@@ -20557,7 +20557,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>platform plan,virtual item,business model,nothing</t>
+          <t>virtual item,platform plan,nothing,business model</t>
         </is>
       </c>
       <c r="E426" t="inlineStr">
@@ -20604,7 +20604,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>nothing,research direction,end-to-end supply chain,information technology,evolution</t>
+          <t>research direction,nothing,end-to-end supply chain,evolution,information technology</t>
         </is>
       </c>
       <c r="E427" t="inlineStr">
@@ -20651,7 +20651,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>mobile compute,majority protocol,gpu compute,nothing,edge compute,mobile application,digital health</t>
+          <t>nothing,digital health,mobile compute,majority protocol,gpu compute,edge compute,mobile application</t>
         </is>
       </c>
       <c r="E428" t="inlineStr">
@@ -20698,7 +20698,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>product recall,counterfeit,serialization,pharmaceutical supply chain,healthcare</t>
+          <t>pharmaceutical supply chain,counterfeit,product recall,serialization,healthcare</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
@@ -20745,7 +20745,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>energy exchange,decentralize market,power exchange,nothing</t>
+          <t>power exchange,decentralize market,energy exchange,nothing</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">
@@ -20795,7 +20795,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>nothing,ethic,transparency,trust,multi-agent system</t>
+          <t>ethic,nothing,multi-agent system,trust,transparency</t>
         </is>
       </c>
       <c r="E431" t="inlineStr">
@@ -20842,7 +20842,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>nothing,IoT,raspberry pi,hyperledger fabric,security</t>
+          <t>nothing,iot,hyperledger fabric,raspberry pi,security</t>
         </is>
       </c>
       <c r="E432" t="inlineStr">
@@ -20889,7 +20889,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>share resource,cryptocurrency,nothing,smart contract,internet 3.0</t>
+          <t>nothing,smart contract,cryptocurrency,internet 3.0,share resource</t>
         </is>
       </c>
       <c r="E433" t="inlineStr">
@@ -20937,7 +20937,7 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>bitcoin,fpga,nothing,physical unclonable function,security</t>
+          <t>fpga,nothing,security,bitcoin,physical unclonable function</t>
         </is>
       </c>
       <c r="E434" t="inlineStr">
@@ -20984,7 +20984,7 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>data trust,security,nothing</t>
+          <t>security,nothing,data trust</t>
         </is>
       </c>
       <c r="E435" t="inlineStr">
@@ -21031,7 +21031,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>power system,nothing,electrical energy trade,bibliometric analysis,security</t>
+          <t>nothing,electrical energy trade,security,bibliometric analysis,power system</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
@@ -21078,7 +21078,7 @@
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>nothing,fashionable product,coordination,supply chain,security</t>
+          <t>supply chain,fashionable product,nothing,security,coordination</t>
         </is>
       </c>
       <c r="E437" t="inlineStr">
@@ -21128,7 +21128,7 @@
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>identity document,security,nothing</t>
+          <t>identity document,nothing,security</t>
         </is>
       </c>
       <c r="E438" t="inlineStr">
@@ -21175,7 +21175,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>reverse logistics,nothing,rfid,tam,characteristic,security</t>
+          <t>nothing,security,reverse logistics,characteristic,tam,rfid</t>
         </is>
       </c>
       <c r="E439" t="inlineStr">
@@ -21269,7 +21269,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>international trade deal,nothing,distribute registry,o38,smart contract,electronic registration,k15,l88,k41,public procurement,к10</t>
+          <t>electronic registration,public procurement,l88,nothing,o38,smart contract,k15,international trade deal,distribute registry,k41,к10</t>
         </is>
       </c>
       <c r="E441" t="inlineStr">
@@ -21316,7 +21316,7 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>cloud storage,third party authenticator,public audit,nothing</t>
+          <t>cloud storage,public audit,third party authenticator,nothing</t>
         </is>
       </c>
       <c r="E442" t="inlineStr">
@@ -21363,7 +21363,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>tax collection,nothing,technology application,management,technology innovation</t>
+          <t>tax collection,nothing,technology innovation,management,technology application</t>
         </is>
       </c>
       <c r="E443" t="inlineStr">
@@ -21410,7 +21410,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>differential game,pigovian tax,dynamic game theory,nothing,bitcoin mine,hamilton–jacobi–bellman equation,nash equilibrium,social optimum,myopic nash equilibrium</t>
+          <t>bitcoin mine,hamilton–jacobi–bellman equation,pigovian tax,dynamic game theory,nothing,nash equilibrium,myopic nash equilibrium,differential game,social optimum</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
@@ -21461,7 +21461,7 @@
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>artificial intelligence,nothing,IoT,decentralise,ttp,security</t>
+          <t>nothing,iot,artificial intelligence,security,ttp,decentralise</t>
         </is>
       </c>
       <c r="E445" t="inlineStr">
@@ -21508,7 +21508,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>smart city,business model,taxonomy,nothing</t>
+          <t>taxonomy,smart city,nothing,business model</t>
         </is>
       </c>
       <c r="E446" t="inlineStr">
@@ -21555,7 +21555,7 @@
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>consensus,pbft,nothing,ibft,poa,cft,fault tolerance</t>
+          <t>cft,consensus,nothing,poa,pbft,fault tolerance,ibft</t>
         </is>
       </c>
       <c r="E447" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>om oracle,bitcoin,consensus,delay,nothing,r</t>
+          <t>consensus,r,nothing,delay,om oracle,bitcoin</t>
         </is>
       </c>
       <c r="E448" t="inlineStr">
@@ -21651,7 +21651,7 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>bitcoin,steganography,behavior,nothing</t>
+          <t>steganography,behavior,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E449" t="inlineStr">
@@ -21699,7 +21699,7 @@
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>disruptive technology,smart contract,nothing</t>
+          <t>smart contract,disruptive technology,nothing</t>
         </is>
       </c>
       <c r="E450" t="inlineStr">
@@ -21749,7 +21749,7 @@
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>money launder,cryptocurrency,nothing,terrorism finance,european parliament,compliance,act,corruption,token economy,liechtenstein,legislation,fatf,security</t>
+          <t>european parliament,nothing,terrorism finance,security,cryptocurrency,money launder,token economy,liechtenstein,act,legislation,fatf,corruption,compliance</t>
         </is>
       </c>
       <c r="E451" t="inlineStr">
@@ -21797,7 +21797,7 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>consensus,nothing,hyperledger,merkle tree,smart contract,decentralize network</t>
+          <t>consensus,decentralize network,nothing,smart contract,merkle tree,hyperledger</t>
         </is>
       </c>
       <c r="E452" t="inlineStr">
@@ -21847,7 +21847,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>nothing,decentralization,privacy,immutable,smart contract</t>
+          <t>privacy,nothing,smart contract,decentralization,immutable</t>
         </is>
       </c>
       <c r="E453" t="inlineStr">
@@ -21894,7 +21894,7 @@
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>consensus,cryptocurrency,cryptography,nothing,decentralization,peer-to-peer network,privacy,cyberspace,smart contract,trust,security</t>
+          <t>privacy,consensus,nothing,smart contract,security,trust,cryptocurrency,decentralization,cryptography,peer-to-peer network,cyberspace</t>
         </is>
       </c>
       <c r="E454" t="inlineStr">
@@ -21941,7 +21941,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>consensus,nothing,multimedia,anonymity,security</t>
+          <t>consensus,multimedia,nothing,security,anonymity</t>
         </is>
       </c>
       <c r="E455" t="inlineStr">
@@ -21992,7 +21992,7 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>privacy,access control,security,nothing</t>
+          <t>access control,privacy,security,nothing</t>
         </is>
       </c>
       <c r="E456" t="inlineStr">
@@ -22086,7 +22086,7 @@
       </c>
       <c r="D458" t="inlineStr">
         <is>
-          <t>st,ardization,system engineer,nothing</t>
+          <t>st,system engineer,ardization,nothing</t>
         </is>
       </c>
       <c r="E458" t="inlineStr">
@@ -22133,7 +22133,7 @@
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,cryptocurrency,nothing</t>
+          <t>consensus,cryptocurrency,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E459" t="inlineStr">
@@ -22180,7 +22180,7 @@
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>decentralization,performance,bite coin,nothing</t>
+          <t>decentralization,bite coin,nothing,performance</t>
         </is>
       </c>
       <c r="E460" t="inlineStr">
@@ -22227,7 +22227,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>nothing,research,citespace,scientometrics,latent dirichlet allocation</t>
+          <t>nothing,citespace,scientometrics,research,latent dirichlet allocation</t>
         </is>
       </c>
       <c r="E461" t="inlineStr">
@@ -22280,7 +22280,7 @@
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>nothing,construction industry,construction contract,technology convergence,cost management</t>
+          <t>cost management,nothing,construction contract,technology convergence,construction industry</t>
         </is>
       </c>
       <c r="E462" t="inlineStr">
@@ -22332,7 +22332,7 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>concept,cryptocurrency,nothing,decentralization,type,issue</t>
+          <t>nothing,cryptocurrency,issue,concept,type,decentralization</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
@@ -22382,7 +22382,7 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>security,smart contract,construction supply chain,taxonomy</t>
+          <t>smart contract,security,construction supply chain,taxonomy</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
@@ -22482,7 +22482,7 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>consensus,nothing,peer-to-peer network,cap theorem</t>
+          <t>consensus,peer-to-peer network,nothing,cap theorem</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -22531,7 +22531,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>nothing,IoT,connect vehicle,smart city,digital technology</t>
+          <t>nothing,iot,smart city,connect vehicle,digital technology</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -22578,7 +22578,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,decentralize,nothing,IoT,ledger,security</t>
+          <t>decentralize,consensus,nothing,iot,ledger,security,bitcoin</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -22629,7 +22629,7 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>consensus,pbft,nothing,hyperledger,poa</t>
+          <t>consensus,nothing,poa,pbft,hyperledger</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
@@ -22676,7 +22676,7 @@
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>bitcoin,n70,l26,n20,nothing,o33,initial coin offer</t>
+          <t>l26,nothing,initial coin offer,n70,o33,bitcoin,n20</t>
         </is>
       </c>
       <c r="E470" t="inlineStr">
@@ -22727,7 +22727,7 @@
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>sustainability,nothing,market,innovation,finance,uae</t>
+          <t>sustainability,nothing,finance,uae,market,innovation</t>
         </is>
       </c>
       <c r="E471" t="inlineStr">
@@ -22821,7 +22821,7 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>rocksdb,nothing,key-value,leveldb,privacy,state,performance,platform</t>
+          <t>privacy,rocksdb,nothing,performance,key-value,leveldb,state,platform</t>
         </is>
       </c>
       <c r="E473" t="inlineStr">
@@ -22869,7 +22869,7 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>consensus,nothing,electoral process,ballot-box,vote system,africa</t>
+          <t>consensus,africa,ballot-box,nothing,electoral process,vote system</t>
         </is>
       </c>
       <c r="E474" t="inlineStr">
@@ -22919,7 +22919,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>security,steep,insurance market,nothing</t>
+          <t>security,steep,nothing,insurance market</t>
         </is>
       </c>
       <c r="E475" t="inlineStr">
@@ -22968,7 +22968,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>smart contract,machine learning,artificial intelligence,nothing</t>
+          <t>smart contract,machine learning,nothing,artificial intelligence</t>
         </is>
       </c>
       <c r="E476" t="inlineStr">
@@ -23015,7 +23015,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>security,IoT,industrial internet of thing,nothing</t>
+          <t>industrial internet of thing,security,nothing,iot</t>
         </is>
       </c>
       <c r="E477" t="inlineStr">
@@ -23063,7 +23063,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>main path analysis,nothing,IoT,healthcare,supply chain</t>
+          <t>main path analysis,supply chain,nothing,iot,healthcare</t>
         </is>
       </c>
       <c r="E478" t="inlineStr">
@@ -23114,7 +23114,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>nothing,e-commerce,hyperledger,reputation system,smart contract</t>
+          <t>reputation system,nothing,smart contract,hyperledger,e-commerce</t>
         </is>
       </c>
       <c r="E479" t="inlineStr">
@@ -23161,7 +23161,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>custom procedure,cross border,nothing</t>
+          <t>cross border,nothing,custom procedure</t>
         </is>
       </c>
       <c r="E480" t="inlineStr">
@@ -23208,7 +23208,7 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>investigation unit,intelligence unit,security,nothing</t>
+          <t>security,intelligence unit,nothing,investigation unit</t>
         </is>
       </c>
       <c r="E481" t="inlineStr">
@@ -23255,7 +23255,7 @@
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>quantum money,quantum cryptography,quantum compute,nothing</t>
+          <t>quantum compute,quantum cryptography,quantum money,nothing</t>
         </is>
       </c>
       <c r="E482" t="inlineStr">
@@ -23304,7 +23304,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>empirical evaluation,smart contract,evaluation framework,nothing</t>
+          <t>smart contract,empirical evaluation,nothing,evaluation framework</t>
         </is>
       </c>
       <c r="E483" t="inlineStr">
@@ -23351,7 +23351,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>tor,cryptography,nothing,pii,privacy,anonymity,onion service,security</t>
+          <t>onion service,privacy,nothing,security,cryptography,tor,pii,anonymity</t>
         </is>
       </c>
       <c r="E484" t="inlineStr">
@@ -23398,7 +23398,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>bitcoin,privacy,cryptography,nothing</t>
+          <t>privacy,cryptography,bitcoin,nothing</t>
         </is>
       </c>
       <c r="E485" t="inlineStr">
@@ -23446,7 +23446,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>healthcare,nothing,security,internet of medical thing</t>
+          <t>security,healthcare,internet of medical thing,nothing</t>
         </is>
       </c>
       <c r="E486" t="inlineStr">
@@ -23493,7 +23493,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>tourism,tourism market,nothing</t>
+          <t>tourism market,tourism,nothing</t>
         </is>
       </c>
       <c r="E487" t="inlineStr">
@@ -23540,7 +23540,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>ehr,interoperability,nothing,healthcare application,security</t>
+          <t>healthcare application,nothing,security,ehr,interoperability</t>
         </is>
       </c>
       <c r="E488" t="inlineStr">
@@ -23683,7 +23683,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>management account,nothing,financial account,technology integration,account information system</t>
+          <t>nothing,account information system,financial account,management account,technology integration</t>
         </is>
       </c>
       <c r="E491" t="inlineStr">
@@ -23730,7 +23730,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>research,systematic map study,nothing</t>
+          <t>systematic map study,research,nothing</t>
         </is>
       </c>
       <c r="E492" t="inlineStr">
@@ -23777,7 +23777,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,nothing,transparency,account,fraud,security</t>
+          <t>account,fraud,nothing,security,cryptocurrency,bitcoin,transparency</t>
         </is>
       </c>
       <c r="E493" t="inlineStr">
@@ -23871,7 +23871,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>smart-contracts,transparency,nothing</t>
+          <t>transparency,smart-contracts,nothing</t>
         </is>
       </c>
       <c r="E495" t="inlineStr">
@@ -23922,7 +23922,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>linddun,stride,security,nothing</t>
+          <t>linddun,nothing,security,stride</t>
         </is>
       </c>
       <c r="E496" t="inlineStr">
@@ -23969,7 +23969,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>nothing,project management,smart contract,construction,supply chain</t>
+          <t>supply chain,nothing,smart contract,project management,construction</t>
         </is>
       </c>
       <c r="E497" t="inlineStr">
@@ -24019,7 +24019,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>uaanet,nothing,manet,uav security,uav</t>
+          <t>manet,nothing,uav,uaanet,uav security</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
@@ -24066,7 +24066,7 @@
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>health 4.0,decentralization,nothing,industry,trust,supply chain,data management,traceability</t>
+          <t>supply chain,data management,nothing,trust,traceability,industry,health 4.0,decentralization</t>
         </is>
       </c>
       <c r="E499" t="inlineStr">
@@ -24113,7 +24113,7 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>poison attack,crypto asset,security,nothing</t>
+          <t>security,poison attack,nothing,crypto asset</t>
         </is>
       </c>
       <c r="E500" t="inlineStr">
@@ -24161,7 +24161,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>healthcare,patient-centred,nothing</t>
+          <t>patient-centred,healthcare,nothing</t>
         </is>
       </c>
       <c r="E501" t="inlineStr">
@@ -24208,7 +24208,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>tow matrix,nothing,disruptive technology,transparency,competitive position,traceability,footwear,supply chain,diffusion of innovation</t>
+          <t>supply chain,nothing,tow matrix,footwear,disruptive technology,competitive position,traceability,diffusion of innovation,transparency</t>
         </is>
       </c>
       <c r="E502" t="inlineStr">
@@ -24255,7 +24255,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>consensus,partition,nothing,certificate authority,sharding,smart contract,public key infrastructure,state machine replication,compute</t>
+          <t>public key infrastructure,consensus,nothing,smart contract,state machine replication,partition,certificate authority,compute,sharding</t>
         </is>
       </c>
       <c r="E503" t="inlineStr">
@@ -24302,7 +24302,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>bank,business model,nothing</t>
+          <t>bank,nothing,business model</t>
         </is>
       </c>
       <c r="E504" t="inlineStr">
@@ -24352,7 +24352,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>systematic map study,nothing,privacy,education,security</t>
+          <t>education,privacy,nothing,security,systematic map study</t>
         </is>
       </c>
       <c r="E505" t="inlineStr">
@@ -24400,7 +24400,7 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>distribute consensus,consensus,security,nothing</t>
+          <t>consensus,security,distribute consensus,nothing</t>
         </is>
       </c>
       <c r="E506" t="inlineStr">
@@ -24500,7 +24500,7 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>bigdata analytics,hash,nothing</t>
+          <t>hash,bigdata analytics,nothing</t>
         </is>
       </c>
       <c r="E508" t="inlineStr">
@@ -24547,7 +24547,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>smart learn environment,open learn ecosystem,inclusion</t>
+          <t>inclusion,smart learn environment,open learn ecosystem</t>
         </is>
       </c>
       <c r="E509" t="inlineStr">
@@ -24688,7 +24688,7 @@
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>nothing,hospitality,network science,tourism management,competitive advantage</t>
+          <t>nothing,network science,competitive advantage,hospitality,tourism management</t>
         </is>
       </c>
       <c r="E512" t="inlineStr">
@@ -24736,7 +24736,7 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>bpmn,nothing,temporal constraint,smart contract,trust,business process</t>
+          <t>nothing,business process,smart contract,trust,temporal constraint,bpmn</t>
         </is>
       </c>
       <c r="E513" t="inlineStr">
@@ -24783,7 +24783,7 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>process choreography,ethereum,reusability,nothing</t>
+          <t>ethereum,reusability,process choreography,nothing</t>
         </is>
       </c>
       <c r="E514" t="inlineStr">
@@ -24877,7 +24877,7 @@
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>energy consumption,cryptocurrency,sustainability,nothing</t>
+          <t>sustainability,cryptocurrency,energy consumption,nothing</t>
         </is>
       </c>
       <c r="E516" t="inlineStr">
@@ -24930,7 +24930,7 @@
       </c>
       <c r="D517" t="inlineStr">
         <is>
-          <t>food supply chain,thematic analysis,nothing</t>
+          <t>thematic analysis,food supply chain,nothing</t>
         </is>
       </c>
       <c r="E517" t="inlineStr">
@@ -24981,7 +24981,7 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>distribute system,consensus,cryptography,decentralize system,nothing</t>
+          <t>consensus,nothing,decentralize system,cryptography,distribute system</t>
         </is>
       </c>
       <c r="E518" t="inlineStr">
@@ -25028,7 +25028,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>ecg feature extraction,artificial intelligence,nothing,IoT,edge compute,ecg monitor,e-health,ubiquitous health,edge ai,ethereum,u-health</t>
+          <t>nothing,iot,artificial intelligence,u-health,ethereum,ecg feature extraction,edge ai,ecg monitor,ubiquitous health,e-health,edge compute</t>
         </is>
       </c>
       <c r="E519" t="inlineStr">
@@ -25075,7 +25075,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>bitcoin,consensus,pseudonymity,cryptocurrency,cryptography,new monetary economics,money,open source,peer-to-peer network,anonymity,censorship resistance,exchange rate indeterminacy,trust,byzantine general problem,security</t>
+          <t>money,consensus,censorship resistance,new monetary economics,exchange rate indeterminacy,open source,security,pseudonymity,trust,cryptocurrency,cryptography,peer-to-peer network,bitcoin,byzantine general problem,anonymity</t>
         </is>
       </c>
       <c r="E520" t="inlineStr"/>

</xml_diff>